<commit_message>
Ajoute les fichiers manquants
</commit_message>
<xml_diff>
--- a/resources/Level1.xlsx
+++ b/resources/Level1.xlsx
@@ -349,7 +349,7 @@
   <dimension ref="A1:BX17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ10" sqref="AJ10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -364,7 +364,7 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2">
-        <f>COUNT(A2:A17)</f>
+        <f>COUNT(A2:A99)</f>
         <v>16</v>
       </c>
       <c r="D1" s="2"/>
@@ -1342,7 +1342,7 @@
         <v>-1</v>
       </c>
       <c r="R6" s="1">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="S6" s="1">
         <v>-1</v>
@@ -1569,7 +1569,7 @@
         <v>-1</v>
       </c>
       <c r="Q7" s="1">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="R7" s="1">
         <v>-1</v>
@@ -1802,7 +1802,7 @@
         <v>-1</v>
       </c>
       <c r="R8" s="1">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="S8" s="1">
         <v>-1</v>
@@ -2029,7 +2029,7 @@
         <v>-1</v>
       </c>
       <c r="Q9" s="1">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="R9" s="1">
         <v>-1</v>
@@ -2462,7 +2462,7 @@
         <v>-1</v>
       </c>
       <c r="H11" s="1">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="I11" s="1">
         <v>-1</v>
@@ -2486,16 +2486,16 @@
         <v>-1</v>
       </c>
       <c r="P11" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Q11" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="R11" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S11" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="T11" s="1">
         <v>-1</v>
@@ -2692,7 +2692,7 @@
         <v>-1</v>
       </c>
       <c r="H12" s="1">
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="I12" s="1">
         <v>-1</v>
@@ -2716,16 +2716,16 @@
         <v>-1</v>
       </c>
       <c r="P12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T12" s="1">
         <v>-1</v>

</xml_diff>